<commit_message>
update ko dính dáng KSCClubBand app
folder db + folder "đề tài". f*ck u
</commit_message>
<xml_diff>
--- a/reference/reference.xlsx
+++ b/reference/reference.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="3030" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>http://demos.telerik.com/kendo-ui/datetimepicker/rangeselection</t>
   </si>
   <si>
     <t>Terelik Kendo UI</t>
+  </si>
+  <si>
+    <t>Time Picker</t>
+  </si>
+  <si>
+    <t>Rome</t>
+  </si>
+  <si>
+    <t>https://github.com/bevacqua/rome</t>
+  </si>
+  <si>
+    <t>Grant</t>
+  </si>
+  <si>
+    <t>http://beginner-sql-tutorial.com/sql-grant-revoke-privileges-roles.htm</t>
+  </si>
+  <si>
+    <t>http://www.mssqlcity.com/articles/adm/sql70roles.htm</t>
+  </si>
+  <si>
+    <t>http://www.techrepublic.com/article/understanding-roles-in-sql-server-security/</t>
+  </si>
+  <si>
+    <t>http://www.mssqltips.com/sqlservertip/2894/understanding-grant-deny-and-revoke-in-sql-server/</t>
   </si>
 </sst>
 </file>
@@ -361,27 +385,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A2:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.140625" customWidth="1"/>
-    <col min="2" max="2" width="115.5703125" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="3" max="3" width="72.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>